<commit_message>
Implemented export data module.
</commit_message>
<xml_diff>
--- a/sql_scripts/verse_passage_records.xlsx
+++ b/sql_scripts/verse_passage_records.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="28800" windowHeight="12570"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="28800" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="37">
   <si>
     <t>', 'Published'),</t>
   </si>
   <si>
-    <t>', 'Published');</t>
-  </si>
-  <si>
     <t>INSERT INTO `verse_passage` (`translation_id`, `chapter_id`, `verse_no`, `passage`, `status`)</t>
   </si>
   <si>
@@ -41,100 +39,103 @@
     <t>, '</t>
   </si>
   <si>
-    <t>The words of king Lemuel, the prophecy that his mother taught him.</t>
-  </si>
-  <si>
-    <t>What, my son? and what, the son of my womb? and what, the son of my vows?</t>
-  </si>
-  <si>
-    <t>Give not thy strength unto women, nor thy ways to that which destroyeth kings.</t>
-  </si>
-  <si>
-    <t>It is not for kings, O Lemuel, it is not for kings to drink wine; nor for princes strong drink:</t>
-  </si>
-  <si>
-    <t>Lest they drink, and forget the law, and pervert the judgment of any of the afflicted.</t>
-  </si>
-  <si>
-    <t>Give strong drink unto him that is ready to perish, and wine unto those that be of heavy hearts.</t>
-  </si>
-  <si>
-    <t>Let him drink, and forget his poverty, and remember his misery no more.</t>
-  </si>
-  <si>
-    <t>Open thy mouth for the dumb in the cause of all such as are appointed to destruction.</t>
-  </si>
-  <si>
-    <t>Open thy mouth, judge righteously, and plead the cause of the poor and needy.</t>
-  </si>
-  <si>
-    <t>Who can find a virtuous woman? for her price is far above rubies.</t>
-  </si>
-  <si>
-    <t>The heart of her husband doth safely trust in her, so that he shall have no need of spoil.</t>
-  </si>
-  <si>
-    <t>She will do him good and not evil all the days of her life.</t>
-  </si>
-  <si>
-    <t>She seeketh wool, and flax, and worketh willingly with her hands.</t>
-  </si>
-  <si>
-    <t>She is like the merchants' ships; she bringeth her food from afar.</t>
-  </si>
-  <si>
-    <t>She riseth also while it is yet night, and giveth meat to her household, and a portion to her maidens.</t>
-  </si>
-  <si>
-    <t>She considereth a field, and buyeth it: with the fruit of her hands she planteth a vineyard.</t>
-  </si>
-  <si>
-    <t>She girdeth her loins with strength, and strengtheneth her arms.</t>
-  </si>
-  <si>
-    <t>She perceiveth that her merchandise is good: her candle goeth not out by night.</t>
-  </si>
-  <si>
-    <t>She layeth her hands to the spindle, and her hands hold the distaff.</t>
-  </si>
-  <si>
-    <t>She stretcheth out her hand to the poor; yea, she reacheth forth her hands to the needy.</t>
-  </si>
-  <si>
-    <t>She is not afraid of the snow for her household: for all her household are clothed with scarlet.</t>
-  </si>
-  <si>
-    <t>She maketh herself coverings of tapestry; her clothing is silk and purple.</t>
-  </si>
-  <si>
-    <t>Her husband is known in the gates, when he sitteth among the elders of the land.</t>
-  </si>
-  <si>
-    <t>She maketh fine linen, and selleth it; and delivereth girdles unto the merchant.</t>
-  </si>
-  <si>
-    <t>Strength and honour are her clothing; and she shall rejoice in time to come.</t>
-  </si>
-  <si>
-    <t>She openeth her mouth with wisdom; and in her tongue is the law of kindness.</t>
-  </si>
-  <si>
-    <t>She looketh well to the ways of her household, and eateth not the bread of idleness.</t>
-  </si>
-  <si>
-    <t>Her children arise up, and call her blessed; her husband also, and he praiseth her.</t>
-  </si>
-  <si>
-    <t>Many daughters have done virtuously, but thou excellest them all.</t>
-  </si>
-  <si>
-    <t>Favour is deceitful, and beauty is vain: but a woman that feareth the Lord, she shall be praised.</t>
-  </si>
-  <si>
-    <t>Give her of the fruit of her hands; and let her own works praise her in the gates.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(5, 31, </t>
+    <t>Proverbs of Solomon. A wise son causeth a father to rejoice, And a foolish son [is] an affliction to his mother.</t>
+  </si>
+  <si>
+    <t>Treasures of wickedness profit not, And righteousness delivereth from death.</t>
+  </si>
+  <si>
+    <t>Jehovah causeth not the soul of the righteous to hunger, And the desire of the wicked He thrusteth away.</t>
+  </si>
+  <si>
+    <t>Poor [is] he who is working -- a slothful hand, And the hand of the diligent maketh rich.</t>
+  </si>
+  <si>
+    <t>Whoso is gathering in summer [is] a wise son, Whoso is sleeping in harvest [is] a son causing shame.</t>
+  </si>
+  <si>
+    <t>Blessings [are] for the head of the righteous, And the mouth of the wicked cover doth violence.</t>
+  </si>
+  <si>
+    <t>The remembrance of the righteous [is] for a blessing, And the name of the wicked doth rot.</t>
+  </si>
+  <si>
+    <t>The wise in heart accepteth commands, And a talkative fool kicketh.</t>
+  </si>
+  <si>
+    <t>Whoso is walking in integrity walketh confidently, And whoso is perverting his ways is known.</t>
+  </si>
+  <si>
+    <t>Whoso is winking the eye giveth grief, And a talkative fool kicketh.</t>
+  </si>
+  <si>
+    <t>A fountain of life [is] the mouth of the righteous, And the mouth of the wicked cover doth violence.</t>
+  </si>
+  <si>
+    <t>Hatred awaketh contentions, And over all transgressions love covereth.</t>
+  </si>
+  <si>
+    <t>In the lips of the intelligent is wisdom found, And a rod [is] for the back of him who is lacking understanding.</t>
+  </si>
+  <si>
+    <t>The wise lay up knowledge, and the mouth of a fool [is] near ruin.</t>
+  </si>
+  <si>
+    <t>The wealth of the rich [is] his strong city, The ruin of the poor [is] their poverty.</t>
+  </si>
+  <si>
+    <t>The wage of the righteous [is] for life, The increase of the wicked for sin.</t>
+  </si>
+  <si>
+    <t>A traveller to life [is] he who is keeping instruction, And whoso is forsaking rebuke is erring.</t>
+  </si>
+  <si>
+    <t>Whoso is covering hatred with lying lips, And whoso is bringing out an evil report is a fool.</t>
+  </si>
+  <si>
+    <t>In the abundance of words transgression ceaseth not, And whoso is restraining his lips [is] wise.</t>
+  </si>
+  <si>
+    <t>The tongue of the righteous [is] chosen silver, The heart of the wicked -- as a little thing.</t>
+  </si>
+  <si>
+    <t>The lips of the righteous delight many, And fools for lack of heart die.</t>
+  </si>
+  <si>
+    <t>The blessing of Jehovah -- it maketh rich, And He addeth no grief with it.</t>
+  </si>
+  <si>
+    <t>To execute inventions [is] as play to a fool, And wisdom to a man of understanding.</t>
+  </si>
+  <si>
+    <t>The feared thing of the wicked it meeteth him, And the desire of the righteous is given.</t>
+  </si>
+  <si>
+    <t>As the passing by of a hurricane, So the wicked is not, And the righteous is a foundation age-during.</t>
+  </si>
+  <si>
+    <t>As vinegar to the teeth, And as smoke to the eyes, So [is] the slothful to those sending him.</t>
+  </si>
+  <si>
+    <t>The fear of Jehovah addeth days, And the years of the wicked are shortened.</t>
+  </si>
+  <si>
+    <t>The hope of the righteous [is] joyful, And the expectation of the wicked perisheth.</t>
+  </si>
+  <si>
+    <t>The way of Jehovah [is] strength to the perfect, And ruin to workers of iniquity.</t>
+  </si>
+  <si>
+    <t>The righteous to the age is not moved, And the wicked inhabit not the earth.</t>
+  </si>
+  <si>
+    <t>The mouth of the righteous uttereth wisdom, And the tongue of frowardness is cut out.</t>
+  </si>
+  <si>
+    <t>The lips of the righteous know a pleasing thing, And the mouth of the wicked perverseness!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2, 10, </t>
   </si>
 </sst>
 </file>
@@ -457,19 +458,22 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F33"/>
+      <selection sqref="A1:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="36.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -480,10 +484,10 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>0</v>
@@ -497,10 +501,10 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>0</v>
@@ -514,10 +518,10 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>0</v>
@@ -531,10 +535,10 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>0</v>
@@ -548,10 +552,10 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>0</v>
@@ -565,10 +569,10 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>0</v>
@@ -582,10 +586,10 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>0</v>
@@ -599,10 +603,10 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>0</v>
@@ -616,10 +620,10 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>0</v>
@@ -633,10 +637,10 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>0</v>
@@ -650,10 +654,10 @@
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>0</v>
@@ -667,10 +671,10 @@
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>0</v>
@@ -684,10 +688,10 @@
         <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>0</v>
@@ -701,10 +705,10 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>0</v>
@@ -718,10 +722,10 @@
         <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>0</v>
@@ -735,10 +739,10 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>0</v>
@@ -752,10 +756,10 @@
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>0</v>
@@ -769,10 +773,10 @@
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>0</v>
@@ -786,10 +790,10 @@
         <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>0</v>
@@ -803,10 +807,10 @@
         <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>0</v>
@@ -820,10 +824,10 @@
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>0</v>
@@ -837,10 +841,10 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>0</v>
@@ -854,10 +858,10 @@
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>0</v>
@@ -871,10 +875,10 @@
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>0</v>
@@ -888,10 +892,10 @@
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>0</v>
@@ -905,10 +909,10 @@
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>0</v>
@@ -922,10 +926,10 @@
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>0</v>
@@ -939,10 +943,10 @@
         <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>0</v>
@@ -956,10 +960,10 @@
         <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>0</v>
@@ -973,10 +977,10 @@
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>0</v>
@@ -990,17 +994,31 @@
         <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34">
+        <v>32</v>
+      </c>
+      <c r="D34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" t="s">
         <v>35</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F35" s="1"/>
@@ -1018,4 +1036,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>